<commit_message>
Finished adding extra columns
</commit_message>
<xml_diff>
--- a/app/static/data/CDMS.xlsx
+++ b/app/static/data/CDMS.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>Email</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>3rd-Payment</t>
+  </si>
+  <si>
+    <t>Extra1</t>
+  </si>
+  <si>
+    <t>Extra2</t>
+  </si>
+  <si>
+    <t>Extra3</t>
   </si>
 </sst>
 </file>
@@ -463,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -474,7 +483,7 @@
     <col min="8" max="8" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -501,6 +510,15 @@
       </c>
       <c r="I1" t="s">
         <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -510,10 +528,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="A2:XFD2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -526,7 +544,7 @@
     <col min="14" max="14" width="9.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -574,6 +592,15 @@
       </c>
       <c r="P1" t="s">
         <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -584,10 +611,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="M1" sqref="M1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -598,7 +625,7 @@
     <col min="11" max="11" width="13.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -634,6 +661,15 @@
       </c>
       <c r="L1" t="s">
         <v>4</v>
+      </c>
+      <c r="M1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>